<commit_message>
add xml test case & change ppt
</commit_message>
<xml_diff>
--- a/test_code/AUI_test/doc/AUI测试用例(TDA4X).xlsx
+++ b/test_code/AUI_test/doc/AUI测试用例(TDA4X).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDY\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4800E5AE-F7C6-4F38-A80F-F800156E5ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBFFD80-A4CB-46DF-80DA-953FEE8C3B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="103">
   <si>
     <t>历史修改记录</t>
   </si>
@@ -722,6 +722,128 @@
       <t>AiControlAndDatamng_test_001</t>
     </r>
     <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3基础层Datamng模块</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DatamngTest_001</t>
+  </si>
+  <si>
+    <t>DatamngTest_002</t>
+  </si>
+  <si>
+    <t>DatamngTest_003</t>
+  </si>
+  <si>
+    <t>xml_document类load_file方法接口测试</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>xml_document类load_file方法接口测试；传入参数文件不存在；预计返回status_file_not_found</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>xml_document类load_file方法接口测试；传入空文件名；预计返回status_file_not_found</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、调用Datamng模块xml_document类load_file方法接口</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>./auitest --gtest_filter=DatamngTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>DatamngTest_001</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>./auitest --gtest_filter=DatamngTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>DatamngTest_002</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>./auitest --gtest_filter=DatamngTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>DatamngTest_003</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
@@ -1321,8 +1443,8 @@
   <dimension ref="A1:O253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1761,8 +1883,12 @@
     </row>
     <row r="16" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>85</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1777,42 +1903,90 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>48</v>
+      </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>